<commit_message>
Scrum and Diary updated Init.java deleted ControllerUI (Link to Medication) and Login.java (Login-Button Design) updated
</commit_message>
<xml_diff>
--- a/doc/Task 9_10/scrum.xlsx
+++ b/doc/Task 9_10/scrum.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="190">
   <si>
     <t>ID</t>
   </si>
@@ -503,15 +503,9 @@
     <t>User Model</t>
   </si>
   <si>
-    <t>Home Site Model</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
-    <t>Implement Home Site (Function Desicion)</t>
-  </si>
-  <si>
     <t>Merge Components</t>
   </si>
   <si>
@@ -566,9 +560,6 @@
     <t>1.4</t>
   </si>
   <si>
-    <t>1.5</t>
-  </si>
-  <si>
     <t>1.6</t>
   </si>
   <si>
@@ -597,6 +588,9 @@
   </si>
   <si>
     <t>Implement the controller for Login and function desicion</t>
+  </si>
+  <si>
+    <t>work in progress</t>
   </si>
 </sst>
 </file>
@@ -787,6 +781,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -805,8 +801,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1033,8 +1027,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="184945280"/>
-        <c:axId val="184967552"/>
+        <c:axId val="161924992"/>
+        <c:axId val="161926528"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1391,11 +1385,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184945280"/>
-        <c:axId val="184967552"/>
+        <c:axId val="161924992"/>
+        <c:axId val="161926528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184945280"/>
+        <c:axId val="161924992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1424,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184967552"/>
+        <c:crossAx val="161926528"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1440,7 +1434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184967552"/>
+        <c:axId val="161926528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1479,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184945280"/>
+        <c:crossAx val="161924992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2238,11 +2232,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -2732,10 +2726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,17 +2787,17 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>187</v>
+      <c r="A2" s="20" t="s">
+        <v>184</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="E2" t="s">
         <v>149</v>
@@ -2818,27 +2812,27 @@
         <v>10</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="L2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>188</v>
+      <c r="A3" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="E3" t="s">
         <v>149</v>
@@ -2853,33 +2847,33 @@
         <v>10</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
+        <v>189</v>
       </c>
       <c r="L3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>177</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" t="s">
         <v>186</v>
       </c>
-      <c r="E4" t="s">
-        <v>189</v>
-      </c>
       <c r="F4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -2891,15 +2885,15 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>178</v>
+      <c r="A5" s="20" t="s">
+        <v>176</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2923,16 +2917,16 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="21"/>
+        <v>189</v>
+      </c>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>179</v>
+      <c r="A6" s="19" t="s">
+        <v>177</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2956,16 +2950,16 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="21"/>
+        <v>189</v>
+      </c>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>180</v>
+      <c r="A7" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2974,10 +2968,10 @@
         <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
         <v>112</v>
@@ -2989,31 +2983,31 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="21"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>181</v>
+      <c r="A8" s="19" t="s">
+        <v>179</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -3025,28 +3019,28 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" s="21"/>
+        <v>189</v>
+      </c>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>182</v>
+      <c r="A9" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
@@ -3060,29 +3054,29 @@
       <c r="K9" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="21"/>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>183</v>
+      <c r="A10" s="20" t="s">
+        <v>181</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -3093,50 +3087,17 @@
       <c r="K10" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="21"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>167</v>
-      </c>
-      <c r="D11" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" t="s">
-        <v>169</v>
-      </c>
-      <c r="F11" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" s="21"/>
+      <c r="L10" s="23"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A21" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L4:L11"/>
+    <mergeCell ref="L4:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3154,32 +3115,32 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="26" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3202,7 +3163,7 @@
       <c r="F4" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
@@ -3516,15 +3477,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>

</xml_diff>

<commit_message>
SCRUM up to date after Sprint1
</commit_message>
<xml_diff>
--- a/doc/Task 9_10/scrum.xlsx
+++ b/doc/Task 9_10/scrum.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9563" windowHeight="2858" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="3" r:id="rId1"/>
@@ -16,12 +16,13 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
+  <oleSize ref="A19:I28"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="192">
   <si>
     <t>ID</t>
   </si>
@@ -398,15 +399,9 @@
     <t>Balance</t>
   </si>
   <si>
-    <t>Daily Completed</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Day</t>
-  </si>
-  <si>
     <t>Planned</t>
   </si>
   <si>
@@ -591,6 +586,18 @@
   </si>
   <si>
     <t>work in progress</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>KW48</t>
+  </si>
+  <si>
+    <t>KW49</t>
+  </si>
+  <si>
+    <t>Weekly Completed</t>
   </si>
 </sst>
 </file>
@@ -803,7 +810,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -822,7 +829,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-CH"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1027,8 +1034,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="161924992"/>
-        <c:axId val="161926528"/>
+        <c:axId val="247705880"/>
+        <c:axId val="247708232"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1385,11 +1392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="161924992"/>
-        <c:axId val="161926528"/>
+        <c:axId val="247705880"/>
+        <c:axId val="247708232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="161924992"/>
+        <c:axId val="247705880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1424,7 +1431,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161926528"/>
+        <c:crossAx val="247708232"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1434,7 +1441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161926528"/>
+        <c:axId val="247708232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1486,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161924992"/>
+        <c:crossAx val="247705880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1932,9 +1939,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1972,9 +1979,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2009,7 +2016,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2044,7 +2051,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2224,14 +2231,14 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
         <v>18</v>
       </c>
@@ -2246,7 +2253,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2257,7 +2264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2268,7 +2275,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2279,7 +2286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2301,7 +2308,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2312,7 +2319,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2323,7 +2330,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2334,7 +2341,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2345,7 +2352,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2356,7 +2363,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2367,7 +2374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2404,19 +2411,19 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.86328125" customWidth="1"/>
+    <col min="2" max="2" width="25.86328125" customWidth="1"/>
+    <col min="3" max="3" width="59.3984375" customWidth="1"/>
+    <col min="4" max="4" width="7.265625" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" customWidth="1"/>
+    <col min="7" max="7" width="10.1328125" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2442,15 +2449,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -2465,7 +2472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2489,7 +2496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2513,7 +2520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2537,7 +2544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2561,7 +2568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2585,7 +2592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2609,7 +2616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2633,7 +2640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2657,7 +2664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2681,7 +2688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2704,7 +2711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2728,27 +2735,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="F3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="4" width="54.86328125" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="18.1328125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.86328125" customWidth="1"/>
+    <col min="12" max="12" width="12.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2783,24 +2790,24 @@
         <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s">
         <v>122</v>
@@ -2812,30 +2819,30 @@
         <v>10</v>
       </c>
       <c r="J2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" t="s">
         <v>115</v>
@@ -2847,33 +2854,33 @@
         <v>10</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>175</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -2882,18 +2889,18 @@
         <v>5</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2902,10 +2909,10 @@
         <v>69</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F5" t="s">
         <v>111</v>
@@ -2917,16 +2924,16 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L5" s="23"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2935,10 +2942,10 @@
         <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F6" t="s">
         <v>113</v>
@@ -2950,28 +2957,28 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L6" s="23"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F7" t="s">
         <v>112</v>
@@ -2983,28 +2990,28 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
       </c>
       <c r="L7" s="23"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F8" t="s">
         <v>111</v>
@@ -3016,28 +3023,28 @@
         <v>5</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L8" s="23"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" t="s">
         <v>161</v>
-      </c>
-      <c r="D9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E9" t="s">
-        <v>163</v>
       </c>
       <c r="F9" t="s">
         <v>113</v>
@@ -3049,31 +3056,31 @@
         <v>5</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K9" t="s">
         <v>8</v>
       </c>
       <c r="L9" s="23"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" t="s">
         <v>165</v>
       </c>
-      <c r="D10" t="s">
-        <v>166</v>
-      </c>
-      <c r="E10" t="s">
-        <v>167</v>
-      </c>
       <c r="F10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -3082,17 +3089,23 @@
         <v>5</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10" t="s">
         <v>8</v>
       </c>
       <c r="L10" s="23"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J12">
+        <f>SUM(J2:J8)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="11"/>
     </row>
   </sheetData>
@@ -3108,15 +3121,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -3129,7 +3142,7 @@
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="25" t="s">
@@ -3141,34 +3154,32 @@
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="B4" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>129</v>
-      </c>
       <c r="E4" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G4" s="26"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>41969</v>
-      </c>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="9"/>
       <c r="B5">
         <v>0</v>
       </c>
@@ -3189,73 +3200,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>178</v>
       </c>
       <c r="F6" s="13">
         <f>IF(D6="",NA(),$F$5-SUM($D$6:D6))</f>
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>175</v>
       </c>
       <c r="F7" s="13">
         <f>IF(D7="",NA(),$F$5-SUM($D$6:D7))</f>
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>170</v>
-      </c>
-      <c r="F8" s="13">
+      <c r="F8" s="13" t="e">
         <f>IF(D8="",NA(),$F$5-SUM($D$6:D8))</f>
-        <v>171</v>
-      </c>
-      <c r="G8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="G8" s="13" t="e">
         <f t="shared" ref="G8:G25" si="1">IF(D8="",NA(),D8)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>4</v>
       </c>
@@ -3268,7 +3276,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>5</v>
       </c>
@@ -3281,7 +3289,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>6</v>
       </c>
@@ -3294,7 +3302,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>7</v>
       </c>
@@ -3307,7 +3315,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>8</v>
       </c>
@@ -3320,7 +3328,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>9</v>
       </c>
@@ -3333,7 +3341,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>10</v>
       </c>
@@ -3346,7 +3354,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>11</v>
       </c>
@@ -3359,7 +3367,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>12</v>
       </c>
@@ -3372,7 +3380,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>13</v>
       </c>
@@ -3385,7 +3393,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>14</v>
       </c>
@@ -3398,7 +3406,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>15</v>
       </c>
@@ -3411,7 +3419,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>16</v>
       </c>
@@ -3424,7 +3432,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>17</v>
       </c>
@@ -3437,7 +3445,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>18</v>
       </c>
@@ -3450,7 +3458,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>19</v>
       </c>
@@ -3463,7 +3471,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>20</v>
       </c>
@@ -3476,9 +3484,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
@@ -3487,17 +3495,17 @@
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:3" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3521,23 +3529,23 @@
       <selection activeCell="L1" sqref="L1:L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="4" width="53.265625" customWidth="1"/>
+    <col min="5" max="5" width="26.73046875" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="18.1328125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.86328125" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3572,7 +3580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -3583,10 +3591,10 @@
         <v>69</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s">
         <v>116</v>
@@ -3604,7 +3612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -3618,7 +3626,7 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F3" t="s">
         <v>116</v>
@@ -3636,7 +3644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -3644,13 +3652,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F4" t="s">
         <v>117</v>
@@ -3668,7 +3676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -3676,16 +3684,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -3700,7 +3708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1.5</v>
       </c>
@@ -3708,16 +3716,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" t="s">
         <v>139</v>
-      </c>
-      <c r="F6" t="s">
-        <v>141</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -3732,7 +3740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1.6</v>
       </c>
@@ -3740,16 +3748,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -3764,7 +3772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1.7</v>
       </c>
@@ -3772,16 +3780,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -3796,7 +3804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2.1</v>
       </c>
@@ -3828,7 +3836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
@@ -3860,7 +3868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>2.2999999999999998</v>
       </c>
@@ -3892,7 +3900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2.4</v>
       </c>
@@ -3924,7 +3932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2.5</v>
       </c>
@@ -3956,7 +3964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2.6</v>
       </c>
@@ -3988,7 +3996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2.7</v>
       </c>
@@ -4020,7 +4028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3.1</v>
       </c>
@@ -4052,7 +4060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>3.2</v>
       </c>
@@ -4084,7 +4092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>3.3</v>
       </c>
@@ -4116,7 +4124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>3.4</v>
       </c>
@@ -4148,7 +4156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
         <v>101</v>
       </c>
@@ -4180,7 +4188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>102</v>
       </c>
@@ -4212,7 +4220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>3.6</v>
       </c>
@@ -4244,7 +4252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>3.8</v>
       </c>
@@ -4276,7 +4284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3.9</v>
       </c>

</xml_diff>

<commit_message>
Updated diary and scrum
</commit_message>
<xml_diff>
--- a/doc/Task 9_10/scrum.xlsx
+++ b/doc/Task 9_10/scrum.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9563" windowHeight="2858" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2865" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="3" r:id="rId1"/>
@@ -16,13 +16,12 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
-  <oleSize ref="A19:I28"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="220">
   <si>
     <t>ID</t>
   </si>
@@ -186,12 +185,6 @@
     <t>User add a new medication plan</t>
   </si>
   <si>
-    <t>Add therapy/tasks/medication</t>
-  </si>
-  <si>
-    <t>User add a new therapy/ tasks/ medication (connect to database)</t>
-  </si>
-  <si>
     <t>Medication info search</t>
   </si>
   <si>
@@ -507,9 +500,6 @@
     <t>Merge the implemented code</t>
   </si>
   <si>
-    <t>UI, controller, models</t>
-  </si>
-  <si>
     <t>Implement User Model with credentials (dummy data)</t>
   </si>
   <si>
@@ -519,9 +509,6 @@
     <t>Implement Database with login data</t>
   </si>
   <si>
-    <t>Model, Database</t>
-  </si>
-  <si>
     <t>GUI Medication</t>
   </si>
   <si>
@@ -585,9 +572,6 @@
     <t>Implement the controller for Login and function desicion</t>
   </si>
   <si>
-    <t>work in progress</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -598,13 +582,112 @@
   </si>
   <si>
     <t>Weekly Completed</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>Login session handling</t>
+  </si>
+  <si>
+    <t>View therapy/tasks/medication</t>
+  </si>
+  <si>
+    <t>User is able to view a new therapy/ tasks/ medication (connect to database)</t>
+  </si>
+  <si>
+    <t>Communication with Database</t>
+  </si>
+  <si>
+    <t>GUI main design</t>
+  </si>
+  <si>
+    <t>Database implementation (dummy XML)</t>
+  </si>
+  <si>
+    <t>Model for medication and therapy</t>
+  </si>
+  <si>
+    <t>All Views</t>
+  </si>
+  <si>
+    <t>XML's for Patients, Therapies, Medication</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>Implement main design (colors, responsive design, icons)</t>
+  </si>
+  <si>
+    <t>Sub total</t>
+  </si>
+  <si>
+    <t>Implement session handling for login</t>
+  </si>
+  <si>
+    <t>Login View</t>
+  </si>
+  <si>
+    <t>Login View / Controller / Auth Model</t>
+  </si>
+  <si>
+    <t>DB Controller / DB Model</t>
+  </si>
+  <si>
+    <t>Implement DB Controller an Model</t>
+  </si>
+  <si>
+    <t>XML Files and Schema</t>
+  </si>
+  <si>
+    <t>Implement models for medication and therapy views</t>
+  </si>
+  <si>
+    <t>Medication View / Therapy View</t>
+  </si>
+  <si>
+    <t>Therapy View</t>
+  </si>
+  <si>
+    <t>Medication View</t>
+  </si>
+  <si>
+    <t>UI / controller / models</t>
+  </si>
+  <si>
+    <t>Model / Database</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +756,14 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -744,7 +835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -788,15 +879,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -808,9 +894,31 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -829,7 +937,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-CH"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1034,8 +1142,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="247705880"/>
-        <c:axId val="247708232"/>
+        <c:axId val="139773824"/>
+        <c:axId val="139775360"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1392,11 +1500,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="247705880"/>
-        <c:axId val="247708232"/>
+        <c:axId val="139773824"/>
+        <c:axId val="139775360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="247705880"/>
+        <c:axId val="139773824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1539,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247708232"/>
+        <c:crossAx val="139775360"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1441,7 +1549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="247708232"/>
+        <c:axId val="139775360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1594,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="247705880"/>
+        <c:crossAx val="139773824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1939,9 +2047,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1979,9 +2087,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2016,7 +2124,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2051,7 +2159,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2231,19 +2339,19 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="17.3984375" customWidth="1"/>
-    <col min="3" max="3" width="20.59765625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -2253,7 +2361,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2264,7 +2372,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2275,7 +2383,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2286,7 +2394,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2297,7 +2405,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2416,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2319,7 +2427,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2330,7 +2438,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2341,7 +2449,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2352,7 +2460,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2363,7 +2471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2374,7 +2482,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2408,22 +2516,22 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.86328125" customWidth="1"/>
-    <col min="2" max="2" width="25.86328125" customWidth="1"/>
-    <col min="3" max="3" width="59.3984375" customWidth="1"/>
-    <col min="4" max="4" width="7.265625" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" customWidth="1"/>
-    <col min="6" max="6" width="13.1328125" customWidth="1"/>
-    <col min="7" max="7" width="10.1328125" customWidth="1"/>
-    <col min="8" max="8" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2449,280 +2557,292 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="B2" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="28">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="H3" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="28">
+        <v>3</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
+        <v>5</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B7" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="28">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>8</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="28">
+        <v>9</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="28">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F11" s="28"/>
+      <c r="G11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="H11" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="28">
+        <v>11</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="H12" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="28">
+        <v>12</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
+      <c r="H13" s="28" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2733,384 +2853,755 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="F3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" customWidth="1"/>
-    <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="32.3984375" customWidth="1"/>
-    <col min="4" max="4" width="54.86328125" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.3984375" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
-    <col min="9" max="9" width="18.1328125" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="16.86328125" customWidth="1"/>
-    <col min="12" max="12" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41" style="2" customWidth="1"/>
+    <col min="4" max="4" width="66.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="20" t="s">
+      <c r="L1" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" s="31"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L6" s="31"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="31"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B2">
+      <c r="E8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L8" s="31"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L9" s="31"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2">
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="27">
+        <f>SUM(H2:H10)</f>
+        <v>55</v>
+      </c>
+      <c r="J11" s="27">
+        <f>SUM(J2:J10)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="30"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="30"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="2">
         <v>10</v>
       </c>
-      <c r="J2">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3">
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>10</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27">
+        <f>SUM(H13:H21)</f>
+        <v>60</v>
+      </c>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27">
+        <f>SUM(J13:J21)</f>
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>187</v>
-      </c>
-      <c r="L3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E4" t="s">
-        <v>184</v>
-      </c>
-      <c r="F4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
-        <v>187</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5" t="s">
-        <v>187</v>
-      </c>
-      <c r="L5" s="23"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6" t="s">
-        <v>187</v>
-      </c>
-      <c r="L6" s="23"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E7" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>3</v>
-      </c>
-      <c r="K7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="23"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8" t="s">
-        <v>187</v>
-      </c>
-      <c r="L8" s="23"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" t="s">
-        <v>161</v>
-      </c>
-      <c r="F9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" s="23"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" t="s">
-        <v>164</v>
-      </c>
-      <c r="E10" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" t="s">
-        <v>172</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L10" s="23"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="J12">
-        <f>SUM(J2:J8)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" s="10"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
+      <c r="K22" s="27"/>
+    </row>
+    <row r="23" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="L4:L10"/>
+    <mergeCell ref="L13:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3121,64 +3612,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26" t="s">
+      <c r="B4" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="E4" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4" s="26"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="9"/>
       <c r="B5">
         <v>0</v>
@@ -3200,9 +3691,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3225,9 +3716,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -3250,7 +3741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>3</v>
       </c>
@@ -3263,7 +3754,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>4</v>
       </c>
@@ -3276,7 +3767,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>5</v>
       </c>
@@ -3289,7 +3780,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>6</v>
       </c>
@@ -3302,7 +3793,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>7</v>
       </c>
@@ -3315,7 +3806,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>8</v>
       </c>
@@ -3328,7 +3819,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>9</v>
       </c>
@@ -3341,7 +3832,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>10</v>
       </c>
@@ -3354,7 +3845,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>11</v>
       </c>
@@ -3367,7 +3858,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>12</v>
       </c>
@@ -3380,7 +3871,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>13</v>
       </c>
@@ -3393,7 +3884,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>14</v>
       </c>
@@ -3406,7 +3897,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>15</v>
       </c>
@@ -3419,7 +3910,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>16</v>
       </c>
@@ -3432,7 +3923,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>17</v>
       </c>
@@ -3445,7 +3936,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>18</v>
       </c>
@@ -3458,7 +3949,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>19</v>
       </c>
@@ -3471,7 +3962,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>20</v>
       </c>
@@ -3484,28 +3975,28 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A27" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
       <c r="C38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3526,23 +4017,23 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L18"/>
+      <selection activeCell="A10" sqref="A10:K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="32.3984375" customWidth="1"/>
-    <col min="4" max="4" width="53.265625" customWidth="1"/>
-    <col min="5" max="5" width="26.73046875" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.3984375" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
-    <col min="9" max="9" width="18.1328125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="16.86328125" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -3588,16 +4079,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -3620,16 +4111,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -3652,16 +4143,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
@@ -3684,16 +4175,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -3716,16 +4207,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" t="s">
         <v>137</v>
-      </c>
-      <c r="F6" t="s">
-        <v>139</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -3748,16 +4239,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -3780,16 +4271,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -3812,16 +4303,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
@@ -3844,16 +4335,16 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
@@ -3876,16 +4367,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G12" t="s">
         <v>5</v>
@@ -3908,16 +4399,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G13" t="s">
         <v>5</v>
@@ -3940,16 +4431,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
@@ -3972,16 +4463,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G15" t="s">
         <v>7</v>
@@ -4004,16 +4495,16 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
@@ -4036,16 +4527,16 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
@@ -4068,16 +4559,16 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -4100,16 +4591,16 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
         <v>6</v>
@@ -4132,16 +4623,16 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>
@@ -4158,22 +4649,22 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G22" t="s">
         <v>7</v>
@@ -4190,22 +4681,22 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G23" t="s">
         <v>7</v>
@@ -4228,16 +4719,16 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G24" t="s">
         <v>6</v>
@@ -4260,16 +4751,16 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G25" t="s">
         <v>7</v>
@@ -4292,16 +4783,16 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Scrum (Sprint Backlog) updated
</commit_message>
<xml_diff>
--- a/doc/Task 9_10/scrum.xlsx
+++ b/doc/Task 9_10/scrum.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="224">
   <si>
     <t>ID</t>
   </si>
@@ -638,6 +638,9 @@
     <t>2.9</t>
   </si>
   <si>
+    <t>2.10</t>
+  </si>
+  <si>
     <t>Implement main design (colors, responsive design, icons)</t>
   </si>
   <si>
@@ -656,18 +659,12 @@
     <t>DB Controller / DB Model</t>
   </si>
   <si>
-    <t>Implement DB Controller an Model</t>
-  </si>
-  <si>
     <t>XML Files and Schema</t>
   </si>
   <si>
     <t>Implement models for medication and therapy views</t>
   </si>
   <si>
-    <t>Medication View / Therapy View</t>
-  </si>
-  <si>
     <t>Therapy View</t>
   </si>
   <si>
@@ -681,6 +678,21 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>Implement DB Controller and Model</t>
+  </si>
+  <si>
+    <t>Controller for therapy</t>
+  </si>
+  <si>
+    <t>Therapy Controller</t>
+  </si>
+  <si>
+    <t>Implement therapy controller with state pattern</t>
+  </si>
+  <si>
+    <t>Medication Model / Therapy Model</t>
   </si>
 </sst>
 </file>
@@ -2578,7 +2590,7 @@
         <v>63</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2853,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3042,7 +3054,7 @@
         <v>152</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>109</v>
@@ -3186,7 +3198,7 @@
         <v>158</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>111</v>
@@ -3222,7 +3234,7 @@
         <v>161</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>168</v>
@@ -3246,7 +3258,7 @@
     </row>
     <row r="11" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="27" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H11" s="27">
         <f>SUM(H2:H10)</f>
@@ -3271,7 +3283,7 @@
         <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>113</v>
@@ -3280,6 +3292,9 @@
         <v>5</v>
       </c>
       <c r="H13" s="2">
+        <v>5</v>
+      </c>
+      <c r="I13" s="2">
         <v>5</v>
       </c>
       <c r="J13" s="2">
@@ -3306,7 +3321,7 @@
         <v>77</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>120</v>
@@ -3315,6 +3330,9 @@
         <v>5</v>
       </c>
       <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2">
         <v>5</v>
       </c>
       <c r="J14" s="2">
@@ -3339,7 +3357,7 @@
         <v>76</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>113</v>
@@ -3348,6 +3366,9 @@
         <v>7</v>
       </c>
       <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="I15" s="2">
         <v>5</v>
       </c>
       <c r="J15" s="2">
@@ -3372,7 +3393,7 @@
         <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>120</v>
@@ -3381,6 +3402,9 @@
         <v>7</v>
       </c>
       <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="I16" s="2">
         <v>5</v>
       </c>
       <c r="J16" s="2">
@@ -3402,10 +3426,10 @@
         <v>194</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>110</v>
@@ -3414,6 +3438,9 @@
         <v>5</v>
       </c>
       <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="I17" s="2">
         <v>5</v>
       </c>
       <c r="J17" s="2">
@@ -3434,13 +3461,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>110</v>
@@ -3449,6 +3476,9 @@
         <v>5</v>
       </c>
       <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
         <v>5</v>
       </c>
       <c r="J18" s="2">
@@ -3457,11 +3487,11 @@
       <c r="K18" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="L18" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>193</v>
-      </c>
       <c r="B19" s="2">
         <v>2</v>
       </c>
@@ -3481,6 +3511,9 @@
         <v>7</v>
       </c>
       <c r="H19" s="2">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2">
         <v>10</v>
       </c>
       <c r="J19" s="2">
@@ -3501,7 +3534,7 @@
         <v>198</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>201</v>
@@ -3513,6 +3546,9 @@
         <v>5</v>
       </c>
       <c r="H20" s="2">
+        <v>10</v>
+      </c>
+      <c r="I20" s="2">
         <v>10</v>
       </c>
       <c r="J20" s="2">
@@ -3536,7 +3572,7 @@
         <v>213</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>109</v>
@@ -3547,6 +3583,9 @@
       <c r="H21" s="2">
         <v>10</v>
       </c>
+      <c r="I21" s="2">
+        <v>10</v>
+      </c>
       <c r="J21" s="2">
         <v>0</v>
       </c>
@@ -3555,10 +3594,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="26" t="s">
+        <v>205</v>
+      </c>
       <c r="B22" s="27"/>
       <c r="C22" s="27" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
@@ -3566,17 +3607,20 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27">
         <f>SUM(H13:H21)</f>
+        <v>55</v>
+      </c>
+      <c r="I22" s="27">
+        <f>SUM(I13:I21)</f>
         <v>60</v>
       </c>
-      <c r="I22" s="27"/>
       <c r="J22" s="27">
         <f>SUM(J13:J21)</f>
         <v>1</v>
       </c>
       <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
     </row>
     <row r="23" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3587,15 +3631,45 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
+      <c r="L23" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L24" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L25" s="2" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2">
+        <v>5</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scrum and diary updated
</commit_message>
<xml_diff>
--- a/doc/Task 9_10/scrum.xlsx
+++ b/doc/Task 9_10/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2865" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2865" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="243">
   <si>
     <t>ID</t>
   </si>
@@ -419,9 +419,6 @@
     <t>Hours</t>
   </si>
   <si>
-    <t>Days</t>
-  </si>
-  <si>
     <t>Grafik</t>
   </si>
   <si>
@@ -693,6 +690,66 @@
   </si>
   <si>
     <t>Medication Model / Therapy Model</t>
+  </si>
+  <si>
+    <t>work in progress</t>
+  </si>
+  <si>
+    <t>KW50</t>
+  </si>
+  <si>
+    <t>KW51</t>
+  </si>
+  <si>
+    <t>KW52</t>
+  </si>
+  <si>
+    <t>KW1</t>
+  </si>
+  <si>
+    <t>KW2</t>
+  </si>
+  <si>
+    <t>KW3</t>
+  </si>
+  <si>
+    <t>KW4</t>
+  </si>
+  <si>
+    <t>KW5</t>
+  </si>
+  <si>
+    <t>KW6</t>
+  </si>
+  <si>
+    <t>KW7</t>
+  </si>
+  <si>
+    <t>KW8</t>
+  </si>
+  <si>
+    <t>KW9</t>
+  </si>
+  <si>
+    <t>KW10</t>
+  </si>
+  <si>
+    <t>KW11</t>
+  </si>
+  <si>
+    <t>KW12</t>
+  </si>
+  <si>
+    <t>KW13</t>
+  </si>
+  <si>
+    <t>KW14</t>
+  </si>
+  <si>
+    <t>KW15</t>
+  </si>
+  <si>
+    <t>Weeks</t>
   </si>
 </sst>
 </file>
@@ -891,21 +948,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -922,11 +964,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -982,11 +1039,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Burndown Chart Example'!$G$3</c:f>
+              <c:f>'Burndown Chart'!$G$3:$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Daily Completed</c:v>
+                  <c:v>Weekly Completed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1074,7 +1131,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[1]Burndown Chart Example'!$G$5:$G$25</c:f>
+              <c:f>'Burndown Chart'!$G$5:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1082,64 +1139,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.25</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.25</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.75</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.75</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1154,8 +1211,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="139773824"/>
-        <c:axId val="139775360"/>
+        <c:axId val="133676416"/>
+        <c:axId val="133686400"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1165,7 +1222,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Burndown Chart Example'!$E$4</c:f>
+              <c:f>'Burndown Chart'!$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1259,72 +1316,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[1]Burndown Chart Example'!$E$5:$E$25</c:f>
+              <c:f>'Burndown Chart'!$E$5:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>315</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>302</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>289</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>276</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>263</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>233</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>199</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>182</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>166</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>149</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>24</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1336,7 +1342,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Burndown Chart Example'!$F$4</c:f>
+              <c:f>'Burndown Chart'!$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1430,72 +1436,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'[1]Burndown Chart Example'!$F$5:$F$25</c:f>
+              <c:f>'Burndown Chart'!$F$5:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>315</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>307</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>292</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>284</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>273.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>261.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>248.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>230.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>222.25</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>214.75</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>202.75</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>194.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>174.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>154.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>137.75</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>137</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>110.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>102.5</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>97</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>95</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,11 +1518,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139773824"/>
-        <c:axId val="139775360"/>
+        <c:axId val="133676416"/>
+        <c:axId val="133686400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139773824"/>
+        <c:axId val="133676416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1557,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139775360"/>
+        <c:crossAx val="133686400"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1561,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139775360"/>
+        <c:axId val="133686400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1612,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139773824"/>
+        <c:crossAx val="133676416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1705,13 +1711,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>69056</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>709613</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>183355</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2359,11 +2365,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -2494,7 +2500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2570,290 +2576,290 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="28" t="s">
-        <v>218</v>
+      <c r="H2" s="23" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="28" t="s">
+      <c r="D4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
-        <v>5</v>
-      </c>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="23">
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="28" t="s">
+      <c r="D6" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="28" t="s">
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28" t="s">
+      <c r="F7" s="23"/>
+      <c r="G7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28" t="s">
+      <c r="F8" s="23"/>
+      <c r="G8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
-        <v>8</v>
-      </c>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="23">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="23"/>
+      <c r="G9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="28" t="s">
+      <c r="D10" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="D11" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="23"/>
+      <c r="G11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28" t="s">
+      <c r="F12" s="23"/>
+      <c r="G12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="H13" s="23" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2867,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,59 +2894,59 @@
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="24" t="s">
-        <v>149</v>
+      <c r="L1" s="19" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>178</v>
+      <c r="A2" s="20" t="s">
+        <v>177</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>120</v>
@@ -2958,27 +2964,27 @@
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>179</v>
+      <c r="A3" s="20" t="s">
+        <v>178</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>113</v>
@@ -2996,30 +3002,30 @@
         <v>8</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>169</v>
+      <c r="A4" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>5</v>
@@ -3034,15 +3040,15 @@
         <v>8</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L4" s="31" t="s">
-        <v>150</v>
+        <v>186</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>170</v>
+      <c r="A5" s="20" t="s">
+        <v>169</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -3051,10 +3057,10 @@
         <v>67</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>109</v>
@@ -3072,13 +3078,13 @@
         <v>5</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L5" s="31"/>
+        <v>186</v>
+      </c>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>171</v>
+      <c r="A6" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -3087,10 +3093,10 @@
         <v>86</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>111</v>
@@ -3108,25 +3114,25 @@
         <v>5</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L6" s="31"/>
+        <v>186</v>
+      </c>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>172</v>
+      <c r="A7" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>110</v>
@@ -3144,25 +3150,25 @@
         <v>3</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L7" s="31"/>
+        <v>186</v>
+      </c>
+      <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>173</v>
+      <c r="A8" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>109</v>
@@ -3180,25 +3186,25 @@
         <v>5</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L8" s="31"/>
+        <v>186</v>
+      </c>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>174</v>
+      <c r="A9" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>111</v>
@@ -3216,28 +3222,28 @@
         <v>5</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L9" s="31"/>
+        <v>186</v>
+      </c>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>175</v>
+      <c r="A10" s="20" t="s">
+        <v>174</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>7</v>
@@ -3252,26 +3258,26 @@
         <v>2</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="L10" s="31"/>
-    </row>
-    <row r="11" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="H11" s="27">
+        <v>186</v>
+      </c>
+      <c r="L10" s="27"/>
+    </row>
+    <row r="11" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="H11" s="22">
         <f>SUM(H2:H10)</f>
         <v>55</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="22">
         <f>SUM(J2:J10)</f>
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>178</v>
+      <c r="A13" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
@@ -3283,7 +3289,7 @@
         <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>113</v>
@@ -3298,18 +3304,18 @@
         <v>5</v>
       </c>
       <c r="J13" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L13" s="30" t="s">
-        <v>195</v>
+        <v>186</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>188</v>
+      <c r="A14" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
@@ -3321,7 +3327,7 @@
         <v>77</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>120</v>
@@ -3336,16 +3342,16 @@
         <v>5</v>
       </c>
       <c r="J14" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L14" s="30"/>
+        <v>223</v>
+      </c>
+      <c r="L14" s="28"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>189</v>
+      <c r="A15" s="21" t="s">
+        <v>188</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -3357,7 +3363,7 @@
         <v>76</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>113</v>
@@ -3377,11 +3383,11 @@
       <c r="K15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="30"/>
+      <c r="L15" s="28"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>190</v>
+      <c r="A16" s="21" t="s">
+        <v>189</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
@@ -3393,7 +3399,7 @@
         <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>120</v>
@@ -3413,23 +3419,23 @@
       <c r="K16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L16" s="30"/>
+      <c r="L16" s="28"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>191</v>
+      <c r="A17" s="21" t="s">
+        <v>190</v>
       </c>
       <c r="B17" s="2">
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>110</v>
@@ -3444,30 +3450,30 @@
         <v>5</v>
       </c>
       <c r="J17" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>8</v>
+        <v>223</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>192</v>
+      <c r="A18" s="21" t="s">
+        <v>191</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>110</v>
@@ -3476,19 +3482,19 @@
         <v>5</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I18" s="2">
         <v>5</v>
       </c>
       <c r="J18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>8</v>
+        <v>223</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -3496,16 +3502,16 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>7</v>
@@ -3517,27 +3523,27 @@
         <v>10</v>
       </c>
       <c r="J19" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>8</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>203</v>
+      <c r="A20" s="21" t="s">
+        <v>202</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>111</v>
@@ -3552,27 +3558,27 @@
         <v>10</v>
       </c>
       <c r="J20" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>8</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>204</v>
+      <c r="A21" s="21" t="s">
+        <v>203</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>109</v>
@@ -3587,40 +3593,40 @@
         <v>10</v>
       </c>
       <c r="J21" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>8</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27">
+      <c r="A22" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22">
         <f>SUM(H13:H21)</f>
-        <v>55</v>
-      </c>
-      <c r="I22" s="27">
+        <v>60</v>
+      </c>
+      <c r="I22" s="22">
         <f>SUM(I13:I21)</f>
         <v>60</v>
       </c>
-      <c r="J22" s="27">
+      <c r="J22" s="22">
         <f>SUM(J13:J21)</f>
-        <v>1</v>
-      </c>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-    </row>
-    <row r="23" spans="1:12" s="27" customFormat="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+    </row>
+    <row r="23" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3631,45 +3637,47 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>5</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L24" s="2" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="B27" s="2">
-        <v>2</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="2">
-        <v>5</v>
-      </c>
-      <c r="J27" s="2">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>8</v>
+      <c r="A27" s="21" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3686,40 +3694,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23" t="s">
-        <v>186</v>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3727,7 +3738,7 @@
         <v>123</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>124</v>
@@ -3741,7 +3752,7 @@
       <c r="F4" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="9"/>
@@ -3767,7 +3778,7 @@
     </row>
     <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3792,7 +3803,7 @@
     </row>
     <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -3815,20 +3826,35 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>224</v>
+      </c>
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="F8" s="13" t="e">
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>175</v>
+      </c>
+      <c r="F8" s="13">
         <f>IF(D8="",NA(),$F$5-SUM($D$6:D8))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G8" s="13" t="e">
+        <v>108</v>
+      </c>
+      <c r="G8" s="13">
         <f t="shared" ref="G8:G25" si="1">IF(D8="",NA(),D8)</f>
-        <v>#N/A</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>225</v>
+      </c>
       <c r="B9">
         <v>4</v>
       </c>
@@ -3842,6 +3868,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>226</v>
+      </c>
       <c r="B10">
         <v>5</v>
       </c>
@@ -3855,6 +3884,9 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>227</v>
+      </c>
       <c r="B11">
         <v>6</v>
       </c>
@@ -3868,6 +3900,9 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>228</v>
+      </c>
       <c r="B12">
         <v>7</v>
       </c>
@@ -3881,6 +3916,9 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>229</v>
+      </c>
       <c r="B13">
         <v>8</v>
       </c>
@@ -3894,6 +3932,9 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>230</v>
+      </c>
       <c r="B14">
         <v>9</v>
       </c>
@@ -3907,6 +3948,9 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>231</v>
+      </c>
       <c r="B15">
         <v>10</v>
       </c>
@@ -3920,6 +3964,9 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>232</v>
+      </c>
       <c r="B16">
         <v>11</v>
       </c>
@@ -3933,6 +3980,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>233</v>
+      </c>
       <c r="B17">
         <v>12</v>
       </c>
@@ -3946,6 +3996,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>234</v>
+      </c>
       <c r="B18">
         <v>13</v>
       </c>
@@ -3958,7 +4011,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>235</v>
+      </c>
       <c r="B19">
         <v>14</v>
       </c>
@@ -3971,7 +4027,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>236</v>
+      </c>
       <c r="B20">
         <v>15</v>
       </c>
@@ -3984,7 +4043,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>237</v>
+      </c>
       <c r="B21">
         <v>16</v>
       </c>
@@ -3997,7 +4059,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>238</v>
+      </c>
       <c r="B22">
         <v>17</v>
       </c>
@@ -4010,7 +4075,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>239</v>
+      </c>
       <c r="B23">
         <v>18</v>
       </c>
@@ -4023,7 +4091,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>240</v>
+      </c>
       <c r="B24">
         <v>19</v>
       </c>
@@ -4036,7 +4107,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>241</v>
+      </c>
       <c r="B25">
         <v>20</v>
       </c>
@@ -4049,28 +4123,28 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>132</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -4156,10 +4230,10 @@
         <v>67</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>114</v>
@@ -4191,7 +4265,7 @@
         <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
         <v>114</v>
@@ -4220,7 +4294,7 @@
         <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" t="s">
         <v>130</v>
@@ -4252,13 +4326,13 @@
         <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E5" t="s">
         <v>130</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
@@ -4281,16 +4355,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" t="s">
         <v>134</v>
       </c>
-      <c r="D6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
-      </c>
       <c r="F6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
@@ -4313,16 +4387,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" t="s">
         <v>147</v>
       </c>
-      <c r="E7" t="s">
-        <v>148</v>
-      </c>
       <c r="F7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -4348,13 +4422,13 @@
         <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
@@ -4625,7 +4699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3.2</v>
       </c>
@@ -4657,7 +4731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3.3</v>
       </c>
@@ -4689,7 +4763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3.4</v>
       </c>
@@ -4721,7 +4795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>99</v>
       </c>
@@ -4753,7 +4827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>100</v>
       </c>
@@ -4785,7 +4859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3.6</v>
       </c>
@@ -4817,7 +4891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3.8</v>
       </c>
@@ -4849,7 +4923,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3.9</v>
       </c>

</xml_diff>

<commit_message>
update scrum after sprint 2
</commit_message>
<xml_diff>
--- a/doc/Task 9_10/scrum.xlsx
+++ b/doc/Task 9_10/scrum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pira\workspace\ch.bfh.btx8081.w2014.blue.git\doc\Task 9_10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2865" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="3" r:id="rId1"/>
@@ -16,12 +21,12 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="246">
   <si>
     <t>ID</t>
   </si>
@@ -674,9 +679,6 @@
     <t>Model / Database</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Implement DB Controller and Model</t>
   </si>
   <si>
@@ -750,6 +752,18 @@
   </si>
   <si>
     <t>Weeks</t>
+  </si>
+  <si>
+    <t>25h</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>working in progress</t>
+  </si>
+  <si>
+    <t>5h</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1001,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1006,7 +1020,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-CH"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1041,7 +1055,7 @@
             <c:strRef>
               <c:f>'Burndown Chart'!$G$3:$G$4</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Weekly Completed</c:v>
                 </c:pt>
@@ -1211,8 +1225,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="133676416"/>
-        <c:axId val="133686400"/>
+        <c:axId val="258423232"/>
+        <c:axId val="258423624"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1518,11 +1532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133676416"/>
-        <c:axId val="133686400"/>
+        <c:axId val="258423232"/>
+        <c:axId val="258423624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133676416"/>
+        <c:axId val="258423232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1557,7 +1571,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133686400"/>
+        <c:crossAx val="258423624"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1581,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133686400"/>
+        <c:axId val="258423624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1612,7 +1626,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133676416"/>
+        <c:crossAx val="258423232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1755,25 +1769,8 @@
             <v>Daily Completed</v>
           </cell>
         </row>
-        <row r="4">
-          <cell r="E4" t="str">
-            <v>Planned</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>Actual</v>
-          </cell>
-        </row>
         <row r="5">
           <cell r="B5">
-            <v>0</v>
-          </cell>
-          <cell r="E5">
-            <v>315</v>
-          </cell>
-          <cell r="F5">
-            <v>315</v>
-          </cell>
-          <cell r="G5">
             <v>0</v>
           </cell>
         </row>
@@ -1781,280 +1778,100 @@
           <cell r="B6">
             <v>1</v>
           </cell>
-          <cell r="E6">
-            <v>302</v>
-          </cell>
-          <cell r="F6">
-            <v>307</v>
-          </cell>
-          <cell r="G6">
-            <v>8</v>
-          </cell>
         </row>
         <row r="7">
           <cell r="B7">
             <v>2</v>
-          </cell>
-          <cell r="E7">
-            <v>289</v>
-          </cell>
-          <cell r="F7">
-            <v>300</v>
-          </cell>
-          <cell r="G7">
-            <v>7</v>
           </cell>
         </row>
         <row r="8">
           <cell r="B8">
             <v>3</v>
           </cell>
-          <cell r="E8">
-            <v>276</v>
-          </cell>
-          <cell r="F8">
-            <v>292</v>
-          </cell>
-          <cell r="G8">
-            <v>8</v>
-          </cell>
         </row>
         <row r="9">
           <cell r="B9">
             <v>4</v>
-          </cell>
-          <cell r="E9">
-            <v>263</v>
-          </cell>
-          <cell r="F9">
-            <v>284</v>
-          </cell>
-          <cell r="G9">
-            <v>8</v>
           </cell>
         </row>
         <row r="10">
           <cell r="B10">
             <v>5</v>
           </cell>
-          <cell r="E10">
-            <v>250</v>
-          </cell>
-          <cell r="F10">
-            <v>273.5</v>
-          </cell>
-          <cell r="G10">
-            <v>10.5</v>
-          </cell>
         </row>
         <row r="11">
           <cell r="B11">
             <v>6</v>
-          </cell>
-          <cell r="E11">
-            <v>233</v>
-          </cell>
-          <cell r="F11">
-            <v>261.5</v>
-          </cell>
-          <cell r="G11">
-            <v>12</v>
           </cell>
         </row>
         <row r="12">
           <cell r="B12">
             <v>7</v>
           </cell>
-          <cell r="E12">
-            <v>216</v>
-          </cell>
-          <cell r="F12">
-            <v>248.5</v>
-          </cell>
-          <cell r="G12">
-            <v>13</v>
-          </cell>
         </row>
         <row r="13">
           <cell r="B13">
             <v>8</v>
-          </cell>
-          <cell r="E13">
-            <v>199</v>
-          </cell>
-          <cell r="F13">
-            <v>230.5</v>
-          </cell>
-          <cell r="G13">
-            <v>18</v>
           </cell>
         </row>
         <row r="14">
           <cell r="B14">
             <v>9</v>
           </cell>
-          <cell r="E14">
-            <v>182</v>
-          </cell>
-          <cell r="F14">
-            <v>222.25</v>
-          </cell>
-          <cell r="G14">
-            <v>8.25</v>
-          </cell>
         </row>
         <row r="15">
           <cell r="B15">
             <v>10</v>
-          </cell>
-          <cell r="E15">
-            <v>166</v>
-          </cell>
-          <cell r="F15">
-            <v>214.75</v>
-          </cell>
-          <cell r="G15">
-            <v>7.5</v>
           </cell>
         </row>
         <row r="16">
           <cell r="B16">
             <v>11</v>
           </cell>
-          <cell r="E16">
-            <v>149</v>
-          </cell>
-          <cell r="F16">
-            <v>202.75</v>
-          </cell>
-          <cell r="G16">
-            <v>12</v>
-          </cell>
         </row>
         <row r="17">
           <cell r="B17">
             <v>12</v>
-          </cell>
-          <cell r="E17">
-            <v>132</v>
-          </cell>
-          <cell r="F17">
-            <v>194.5</v>
-          </cell>
-          <cell r="G17">
-            <v>8.25</v>
           </cell>
         </row>
         <row r="18">
           <cell r="B18">
             <v>13</v>
           </cell>
-          <cell r="E18">
-            <v>115</v>
-          </cell>
-          <cell r="F18">
-            <v>174.5</v>
-          </cell>
-          <cell r="G18">
-            <v>20</v>
-          </cell>
         </row>
         <row r="19">
           <cell r="B19">
             <v>14</v>
-          </cell>
-          <cell r="E19">
-            <v>98</v>
-          </cell>
-          <cell r="F19">
-            <v>154.5</v>
-          </cell>
-          <cell r="G19">
-            <v>20</v>
           </cell>
         </row>
         <row r="20">
           <cell r="B20">
             <v>15</v>
           </cell>
-          <cell r="E20">
-            <v>80</v>
-          </cell>
-          <cell r="F20">
-            <v>137.75</v>
-          </cell>
-          <cell r="G20">
-            <v>16.75</v>
-          </cell>
         </row>
         <row r="21">
           <cell r="B21">
             <v>16</v>
-          </cell>
-          <cell r="E21">
-            <v>64</v>
-          </cell>
-          <cell r="F21">
-            <v>137</v>
-          </cell>
-          <cell r="G21">
-            <v>0.75</v>
           </cell>
         </row>
         <row r="22">
           <cell r="B22">
             <v>17</v>
           </cell>
-          <cell r="E22">
-            <v>48</v>
-          </cell>
-          <cell r="F22">
-            <v>110.5</v>
-          </cell>
-          <cell r="G22">
-            <v>26.5</v>
-          </cell>
         </row>
         <row r="23">
           <cell r="B23">
             <v>18</v>
-          </cell>
-          <cell r="E23">
-            <v>40</v>
-          </cell>
-          <cell r="F23">
-            <v>102.5</v>
-          </cell>
-          <cell r="G23">
-            <v>8</v>
           </cell>
         </row>
         <row r="24">
           <cell r="B24">
             <v>19</v>
           </cell>
-          <cell r="E24">
-            <v>32</v>
-          </cell>
-          <cell r="F24">
-            <v>97</v>
-          </cell>
-          <cell r="G24">
-            <v>5.5</v>
-          </cell>
         </row>
         <row r="25">
           <cell r="B25">
             <v>20</v>
-          </cell>
-          <cell r="E25">
-            <v>24</v>
-          </cell>
-          <cell r="F25">
-            <v>95</v>
-          </cell>
-          <cell r="G25">
-            <v>2</v>
           </cell>
         </row>
       </sheetData>
@@ -2065,9 +1882,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2105,9 +1922,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2142,7 +1959,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2177,7 +1994,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2357,11 +2174,11 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
@@ -2379,7 +2196,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2390,7 +2207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2401,7 +2218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2412,7 +2229,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2423,7 +2240,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2434,7 +2251,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2262,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2456,7 +2273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2467,7 +2284,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2478,7 +2295,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2489,7 +2306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2500,7 +2317,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2533,23 +2350,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.86328125" customWidth="1"/>
+    <col min="2" max="2" width="25.86328125" customWidth="1"/>
+    <col min="3" max="3" width="61.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" customWidth="1"/>
+    <col min="7" max="7" width="10.1328125" customWidth="1"/>
+    <col min="8" max="8" width="16.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2575,7 +2392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -2591,15 +2408,17 @@
       <c r="E2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="23"/>
+      <c r="F2" s="23" t="s">
+        <v>242</v>
+      </c>
       <c r="G2" s="23" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="23">
         <v>2</v>
       </c>
@@ -2623,7 +2442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="23">
         <v>3</v>
       </c>
@@ -2639,15 +2458,17 @@
       <c r="E4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="G4" s="23" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="23">
         <v>4</v>
       </c>
@@ -2663,15 +2484,17 @@
       <c r="E5" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="G5" s="23" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="23">
         <v>5</v>
       </c>
@@ -2687,15 +2510,17 @@
       <c r="E6" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="23" t="s">
+        <v>243</v>
+      </c>
       <c r="G6" s="23" t="s">
-        <v>17</v>
+        <v>243</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="23">
         <v>6</v>
       </c>
@@ -2711,15 +2536,17 @@
       <c r="E7" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="23" t="s">
+        <v>66</v>
+      </c>
       <c r="G7" s="23" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="23">
         <v>7</v>
       </c>
@@ -2735,15 +2562,17 @@
       <c r="E8" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="23" t="s">
+        <v>243</v>
+      </c>
       <c r="G8" s="23" t="s">
-        <v>17</v>
+        <v>243</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="23">
         <v>8</v>
       </c>
@@ -2759,15 +2588,17 @@
       <c r="E9" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="G9" s="23" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="23">
         <v>9</v>
       </c>
@@ -2783,15 +2614,17 @@
       <c r="E10" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>245</v>
+      </c>
       <c r="G10" s="23" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="23">
         <v>10</v>
       </c>
@@ -2815,7 +2648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="23">
         <v>11</v>
       </c>
@@ -2831,15 +2664,17 @@
       <c r="E12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="23"/>
+      <c r="F12" s="23" t="s">
+        <v>245</v>
+      </c>
       <c r="G12" s="23" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="23">
         <v>12</v>
       </c>
@@ -2873,28 +2708,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="D7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.1328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="7" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="4" width="66.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.06640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.796875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2932,7 +2767,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="20" t="s">
         <v>177</v>
       </c>
@@ -2970,7 +2805,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
         <v>178</v>
       </c>
@@ -3008,7 +2843,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="21" t="s">
         <v>168</v>
       </c>
@@ -3046,7 +2881,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="20" t="s">
         <v>169</v>
       </c>
@@ -3082,7 +2917,7 @@
       </c>
       <c r="L5" s="27"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="21" t="s">
         <v>170</v>
       </c>
@@ -3118,7 +2953,7 @@
       </c>
       <c r="L6" s="27"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="21" t="s">
         <v>171</v>
       </c>
@@ -3154,7 +2989,7 @@
       </c>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="21" t="s">
         <v>172</v>
       </c>
@@ -3190,7 +3025,7 @@
       </c>
       <c r="L8" s="27"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="21" t="s">
         <v>173</v>
       </c>
@@ -3226,7 +3061,7 @@
       </c>
       <c r="L9" s="27"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>174</v>
       </c>
@@ -3262,7 +3097,7 @@
       </c>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C11" s="22" t="s">
         <v>206</v>
       </c>
@@ -3275,7 +3110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="21" t="s">
         <v>177</v>
       </c>
@@ -3313,7 +3148,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="21" t="s">
         <v>187</v>
       </c>
@@ -3345,11 +3180,11 @@
         <v>3</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L14" s="28"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
         <v>188</v>
       </c>
@@ -3378,14 +3213,14 @@
         <v>5</v>
       </c>
       <c r="J15" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>8</v>
+        <v>222</v>
       </c>
       <c r="L15" s="28"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="21" t="s">
         <v>189</v>
       </c>
@@ -3414,14 +3249,14 @@
         <v>5</v>
       </c>
       <c r="J16" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>8</v>
+        <v>222</v>
       </c>
       <c r="L16" s="28"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="21" t="s">
         <v>190</v>
       </c>
@@ -3450,16 +3285,16 @@
         <v>5</v>
       </c>
       <c r="J17" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="21" t="s">
         <v>191</v>
       </c>
@@ -3467,13 +3302,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>110</v>
@@ -3488,16 +3323,16 @@
         <v>5</v>
       </c>
       <c r="J18" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B19" s="2">
         <v>2</v>
       </c>
@@ -3523,13 +3358,13 @@
         <v>10</v>
       </c>
       <c r="J19" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="21" t="s">
         <v>202</v>
       </c>
@@ -3558,13 +3393,13 @@
         <v>10</v>
       </c>
       <c r="J20" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="21" t="s">
         <v>203</v>
       </c>
@@ -3578,7 +3413,7 @@
         <v>212</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>109</v>
@@ -3593,13 +3428,13 @@
         <v>10</v>
       </c>
       <c r="J21" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="21" t="s">
         <v>204</v>
       </c>
@@ -3621,12 +3456,12 @@
       </c>
       <c r="J22" s="22">
         <f>SUM(J13:J21)</f>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3638,7 +3473,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B24" s="2">
         <v>3</v>
       </c>
@@ -3646,7 +3481,7 @@
         <v>196</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>210</v>
@@ -3670,12 +3505,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="L25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="21" t="s">
         <v>192</v>
       </c>
@@ -3694,13 +3529,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
@@ -3718,7 +3553,7 @@
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="30" t="s">
@@ -3733,7 +3568,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>123</v>
       </c>
@@ -3754,7 +3589,7 @@
       </c>
       <c r="G4" s="31"/>
     </row>
-    <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9"/>
       <c r="B5">
         <v>0</v>
@@ -3776,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>183</v>
       </c>
@@ -3801,7 +3636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>184</v>
       </c>
@@ -3826,9 +3661,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -3851,9 +3686,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -3867,9 +3702,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -3883,9 +3718,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -3899,9 +3734,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -3915,9 +3750,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -3931,9 +3766,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -3947,9 +3782,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -3963,9 +3798,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -3979,9 +3814,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -3995,9 +3830,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B18">
         <v>13</v>
@@ -4011,9 +3846,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B19">
         <v>14</v>
@@ -4027,9 +3862,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B20">
         <v>15</v>
@@ -4043,9 +3878,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B21">
         <v>16</v>
@@ -4059,9 +3894,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B22">
         <v>17</v>
@@ -4075,9 +3910,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -4091,9 +3926,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B24">
         <v>19</v>
@@ -4107,9 +3942,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B25">
         <v>20</v>
@@ -4123,7 +3958,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="29" t="s">
         <v>132</v>
       </c>
@@ -4134,17 +3969,17 @@
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="17"/>
     </row>
-    <row r="33" spans="1:3" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4168,23 +4003,23 @@
       <selection activeCell="A10" sqref="A10:K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="4" width="53.265625" customWidth="1"/>
+    <col min="5" max="5" width="26.73046875" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" customWidth="1"/>
+    <col min="8" max="8" width="17.1328125" customWidth="1"/>
+    <col min="9" max="9" width="18.1328125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.86328125" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4219,7 +4054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -4251,7 +4086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -4283,7 +4118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -4315,7 +4150,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -4347,7 +4182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1.5</v>
       </c>
@@ -4379,7 +4214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1.6</v>
       </c>
@@ -4411,7 +4246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1.7</v>
       </c>
@@ -4443,7 +4278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2.1</v>
       </c>
@@ -4475,7 +4310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
@@ -4507,7 +4342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>2.2999999999999998</v>
       </c>
@@ -4539,7 +4374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2.4</v>
       </c>
@@ -4571,7 +4406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2.5</v>
       </c>
@@ -4603,7 +4438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2.6</v>
       </c>
@@ -4635,7 +4470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2.7</v>
       </c>
@@ -4667,7 +4502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3.1</v>
       </c>
@@ -4699,7 +4534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>3.2</v>
       </c>
@@ -4731,7 +4566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>3.3</v>
       </c>
@@ -4763,7 +4598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>3.4</v>
       </c>
@@ -4795,7 +4630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
         <v>99</v>
       </c>
@@ -4827,7 +4662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>100</v>
       </c>
@@ -4859,7 +4694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>3.6</v>
       </c>
@@ -4891,7 +4726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>3.8</v>
       </c>
@@ -4923,7 +4758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3.9</v>
       </c>

</xml_diff>

<commit_message>
Diary updated, StatePattern diagram uploaded, scrum updated
</commit_message>
<xml_diff>
--- a/doc/Task 9_10/scrum.xlsx
+++ b/doc/Task 9_10/scrum.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pira\workspace\ch.bfh.btx8081.w2014.blue.git\doc\Task 9_10\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2865" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2865" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="3" r:id="rId1"/>
@@ -21,12 +16,46 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stefan Johner</author>
+  </authors>
+  <commentList>
+    <comment ref="L2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stefan Johner:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Zuordnung der User Stories noch überarbeiten!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="240">
   <si>
     <t>ID</t>
   </si>
@@ -715,42 +744,6 @@
     <t>KW3</t>
   </si>
   <si>
-    <t>KW4</t>
-  </si>
-  <si>
-    <t>KW5</t>
-  </si>
-  <si>
-    <t>KW6</t>
-  </si>
-  <si>
-    <t>KW7</t>
-  </si>
-  <si>
-    <t>KW8</t>
-  </si>
-  <si>
-    <t>KW9</t>
-  </si>
-  <si>
-    <t>KW10</t>
-  </si>
-  <si>
-    <t>KW11</t>
-  </si>
-  <si>
-    <t>KW12</t>
-  </si>
-  <si>
-    <t>KW13</t>
-  </si>
-  <si>
-    <t>KW14</t>
-  </si>
-  <si>
-    <t>KW15</t>
-  </si>
-  <si>
     <t>Weeks</t>
   </si>
   <si>
@@ -764,13 +757,31 @@
   </si>
   <si>
     <t>5h</t>
+  </si>
+  <si>
+    <t>Tester classes</t>
+  </si>
+  <si>
+    <t>Patient summary report in GUI HomeView</t>
+  </si>
+  <si>
+    <t>Back Buttons in all GUI Views</t>
+  </si>
+  <si>
+    <t>Daily medication</t>
+  </si>
+  <si>
+    <t>Revise exception handling</t>
+  </si>
+  <si>
+    <t>KW47</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,8 +859,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -878,6 +902,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
         <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -940,14 +970,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -984,12 +1012,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -999,9 +1021,21 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1020,7 +1054,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-CH"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1055,7 +1089,7 @@
             <c:strRef>
               <c:f>'Burndown Chart'!$G$3:$G$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Weekly Completed</c:v>
                 </c:pt>
@@ -1145,10 +1179,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$G$5:$G$25</c:f>
+              <c:f>'Burndown Chart'!$G$5:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1159,58 +1193,22 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>#N/A</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1225,8 +1223,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="50"/>
-        <c:axId val="258423232"/>
-        <c:axId val="258423624"/>
+        <c:axId val="177907200"/>
+        <c:axId val="177908736"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1330,21 +1328,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$E$5:$E$25</c:f>
+              <c:f>'Burndown Chart'!$E$5:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>178</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>175</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>175</c:v>
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1450,10 +1463,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$F$5:$F$25</c:f>
+              <c:f>'Burndown Chart'!$F$5:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>180</c:v>
                 </c:pt>
@@ -1464,58 +1477,22 @@
                   <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1532,11 +1509,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="258423232"/>
-        <c:axId val="258423624"/>
+        <c:axId val="177907200"/>
+        <c:axId val="177908736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="258423232"/>
+        <c:axId val="177907200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,7 +1548,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="258423624"/>
+        <c:crossAx val="177908736"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1581,7 +1558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="258423624"/>
+        <c:axId val="177908736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,7 +1603,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="258423232"/>
+        <c:crossAx val="177907200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1723,15 +1700,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>69056</xdr:rowOff>
+      <xdr:colOff>80963</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>164308</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>709613</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>183355</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>88107</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1882,9 +1859,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1922,9 +1899,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1959,7 +1936,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1994,7 +1971,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2174,19 +2151,19 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="17.3984375" customWidth="1"/>
-    <col min="3" max="3" width="20.59765625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -2196,7 +2173,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2207,7 +2184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2218,7 +2195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2229,7 +2206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2240,7 +2217,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2251,7 +2228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2262,7 +2239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2273,7 +2250,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2284,7 +2261,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2295,7 +2272,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2306,7 +2283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2317,7 +2294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2350,20 +2327,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.86328125" customWidth="1"/>
-    <col min="2" max="2" width="25.86328125" customWidth="1"/>
-    <col min="3" max="3" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1328125" customWidth="1"/>
-    <col min="7" max="7" width="10.1328125" customWidth="1"/>
-    <col min="8" max="8" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
@@ -2392,309 +2369,309 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="23">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="23" t="s">
+      <c r="D2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="G2" s="23" t="s">
+      <c r="F2" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="23">
+    <row r="3" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="23">
+    <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="23" t="s">
+      <c r="D4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="23">
+    <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="23" t="s">
+      <c r="D5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="23">
-        <v>5</v>
-      </c>
-      <c r="B6" s="23" t="s">
+    <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="21">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="23" t="s">
+      <c r="D6" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="23">
+      <c r="F6" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="23" t="s">
+      <c r="D7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="23">
+      <c r="H7" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="23">
+      <c r="F8" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="23">
+    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="23">
+      <c r="F10" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="23" t="s">
+      <c r="D11" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23" t="s">
+      <c r="F11" s="21"/>
+      <c r="G11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="23">
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="23">
+      <c r="F12" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="21">
         <v>12</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23" t="s">
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="21" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2705,70 +2682,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="7" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.06640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
+    <row r="1" spans="1:12" s="17" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="17" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="18" t="s">
         <v>177</v>
       </c>
       <c r="B2" s="2">
@@ -2801,12 +2778,12 @@
       <c r="K2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="28" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="18" t="s">
         <v>178</v>
       </c>
       <c r="B3" s="2">
@@ -2839,12 +2816,12 @@
       <c r="K3" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="28" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>168</v>
       </c>
       <c r="B4" s="2">
@@ -2877,12 +2854,12 @@
       <c r="K4" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="29" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B5" s="2">
@@ -2915,10 +2892,10 @@
       <c r="K5" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L5" s="27"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="21" t="s">
+      <c r="L5" s="29"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>170</v>
       </c>
       <c r="B6" s="2">
@@ -2951,10 +2928,10 @@
       <c r="K6" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L6" s="27"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="21" t="s">
+      <c r="L6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>171</v>
       </c>
       <c r="B7" s="2">
@@ -2987,10 +2964,10 @@
       <c r="K7" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L7" s="27"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="21" t="s">
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>172</v>
       </c>
       <c r="B8" s="2">
@@ -3023,10 +3000,10 @@
       <c r="K8" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="21" t="s">
+      <c r="L8" s="29"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>173</v>
       </c>
       <c r="B9" s="2">
@@ -3059,10 +3036,10 @@
       <c r="K9" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="20" t="s">
+      <c r="L9" s="29"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>174</v>
       </c>
       <c r="B10" s="2">
@@ -3095,23 +3072,31 @@
       <c r="K10" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="22" t="s">
+      <c r="L10" s="29"/>
+    </row>
+    <row r="11" spans="1:12" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="C11" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="20">
         <f>SUM(H2:H10)</f>
         <v>55</v>
       </c>
-      <c r="J11" s="22">
+      <c r="I11" s="20">
+        <f>SUM(I2:I10)</f>
+        <v>49</v>
+      </c>
+      <c r="J11" s="20">
         <f>SUM(J2:J10)</f>
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="21" t="s">
+      <c r="L11" s="30"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="28"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>177</v>
       </c>
       <c r="B13" s="2">
@@ -3144,12 +3129,12 @@
       <c r="K13" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="31" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" s="21" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>187</v>
       </c>
       <c r="B14" s="2">
@@ -3182,10 +3167,10 @@
       <c r="K14" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="21" t="s">
+      <c r="L14" s="31"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>188</v>
       </c>
       <c r="B15" s="2">
@@ -3218,10 +3203,10 @@
       <c r="K15" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" s="21" t="s">
+      <c r="L15" s="31"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>189</v>
       </c>
       <c r="B16" s="2">
@@ -3254,10 +3239,10 @@
       <c r="K16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="21" t="s">
+      <c r="L16" s="31"/>
+    </row>
+    <row r="17" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A17" s="19" t="s">
         <v>190</v>
       </c>
       <c r="B17" s="2">
@@ -3290,12 +3275,12 @@
       <c r="K17" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="28" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="21" t="s">
+    <row r="18" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A18" s="19" t="s">
         <v>191</v>
       </c>
       <c r="B18" s="2">
@@ -3323,16 +3308,16 @@
         <v>5</v>
       </c>
       <c r="J18" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="L18" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L18" s="28" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B19" s="2">
         <v>2</v>
       </c>
@@ -3363,9 +3348,10 @@
       <c r="K19" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="21" t="s">
+      <c r="L19" s="28"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A20" s="19" t="s">
         <v>202</v>
       </c>
       <c r="B20" s="2">
@@ -3398,9 +3384,10 @@
       <c r="K20" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="21" t="s">
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A21" s="19" t="s">
         <v>203</v>
       </c>
       <c r="B21" s="2">
@@ -3433,86 +3420,398 @@
       <c r="K21" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="21" t="s">
+      <c r="L21" s="28"/>
+    </row>
+    <row r="22" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A22" s="19"/>
+      <c r="D22" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L22" s="28"/>
+    </row>
+    <row r="23" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22">
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20">
         <f>SUM(H13:H21)</f>
         <v>60</v>
       </c>
-      <c r="I22" s="22">
-        <f>SUM(I13:I21)</f>
+      <c r="I23" s="20">
+        <f>SUM(I13:I22)</f>
+        <v>62</v>
+      </c>
+      <c r="J23" s="20">
+        <f>SUM(J13:J22)</f>
         <v>60</v>
       </c>
-      <c r="J22" s="22">
-        <f>SUM(J13:J21)</f>
+      <c r="K23" s="20"/>
+      <c r="L23" s="30"/>
+    </row>
+    <row r="24" spans="1:12" s="20" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="30"/>
+    </row>
+    <row r="25" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="2">
+        <v>5</v>
+      </c>
+      <c r="I25" s="2">
+        <v>4</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="D26" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>3</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L26" s="28"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>3</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L27" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L28" s="28"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>3</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L29" s="28"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L30" s="28"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="2">
+        <v>18</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L31" s="28"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>2</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L32" s="28"/>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="2">
+        <v>10</v>
+      </c>
+      <c r="I33" s="2">
+        <v>12</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L33" s="28"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="2">
+        <v>15</v>
+      </c>
+      <c r="I34" s="2">
+        <v>16</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L34" s="28"/>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="2">
+        <v>10</v>
+      </c>
+      <c r="I35" s="2">
+        <v>12</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L35" s="28"/>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H36" s="20">
+        <f>SUM(H25:H35)</f>
         <v>60</v>
       </c>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-    </row>
-    <row r="23" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B24" s="2">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="L25" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="21" t="s">
-        <v>192</v>
+      <c r="I36" s="20">
+        <f>SUM(I25:I35)</f>
+        <v>64</v>
+      </c>
+      <c r="J36" s="20">
+        <f>SUM(J25:J35)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3522,469 +3821,333 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="30" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="31"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="9"/>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
         <v>180</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <v>180</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="11">
         <f t="shared" ref="G5:G7" si="0">IF(D5="",NA(),D5)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="11">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="11">
         <v>21</v>
       </c>
-      <c r="E6">
-        <v>178</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="E6" s="11">
+        <f>E5-C6</f>
+        <v>150</v>
+      </c>
+      <c r="F6" s="11">
         <f>IF(D6="",NA(),$F$5-SUM($D$6:D6))</f>
         <v>159</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="11">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="11">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="11">
         <v>21</v>
       </c>
-      <c r="E7">
-        <v>175</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="E7" s="11">
+        <f t="shared" ref="E7:E13" si="1">E6-C7</f>
+        <v>120</v>
+      </c>
+      <c r="F7" s="11">
         <f>IF(D7="",NA(),$F$5-SUM($D$6:D7))</f>
         <v>138</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="11">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="11">
         <v>30</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="11">
+        <v>20</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="F8" s="11">
+        <f>IF(D8="",NA(),$F$5-SUM($D$6:D8))</f>
+        <v>118</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" ref="G8:G13" si="2">IF(D8="",NA(),D8)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" s="11">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11">
         <v>30</v>
       </c>
-      <c r="E8">
-        <v>175</v>
-      </c>
-      <c r="F8" s="13">
-        <f>IF(D8="",NA(),$F$5-SUM($D$6:D8))</f>
-        <v>108</v>
-      </c>
-      <c r="G8" s="13">
-        <f t="shared" ref="G8:G25" si="1">IF(D8="",NA(),D8)</f>
+      <c r="D9" s="11">
+        <v>20</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="F9" s="11">
+        <f>IF(D9="",NA(),$F$5-SUM($D$6:D9))</f>
+        <v>98</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="11">
+        <v>5</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11">
+        <v>13</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="F10" s="11">
+        <f>IF(D10="",NA(),$F$5-SUM($D$6:D10))</f>
+        <v>85</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="11">
+        <v>6</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="F9" s="13" t="e">
-        <f>IF(D9="",NA(),$F$5-SUM($D$6:D9))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G9" s="13" t="e">
+      <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>225</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="F10" s="13" t="e">
-        <f>IF(D10="",NA(),$F$5-SUM($D$6:D10))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G10" s="13" t="e">
+        <v>60</v>
+      </c>
+      <c r="F11" s="11">
+        <f>IF(D11="",NA(),$F$5-SUM($D$6:D11))</f>
+        <v>55</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" s="11">
+        <v>7</v>
+      </c>
+      <c r="C12" s="11">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11">
+        <v>20</v>
+      </c>
+      <c r="E12" s="11">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>226</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="F11" s="13" t="e">
-        <f>IF(D11="",NA(),$F$5-SUM($D$6:D11))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G11" s="13" t="e">
+        <v>30</v>
+      </c>
+      <c r="F12" s="11">
+        <f>IF(D12="",NA(),$F$5-SUM($D$6:D12))</f>
+        <v>35</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="11">
+        <v>8</v>
+      </c>
+      <c r="C13" s="11">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11">
+        <v>35</v>
+      </c>
+      <c r="E13" s="11">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>227</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="F12" s="13" t="e">
-        <f>IF(D12="",NA(),$F$5-SUM($D$6:D12))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G12" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>228</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="F13" s="13" t="e">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
         <f>IF(D13="",NA(),$F$5-SUM($D$6:D13))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G13" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A15" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.45">
+      <c r="A21" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="C26" t="s">
         <v>229</v>
-      </c>
-      <c r="B14">
-        <v>9</v>
-      </c>
-      <c r="F14" s="13" t="e">
-        <f>IF(D14="",NA(),$F$5-SUM($D$6:D14))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G14" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>230</v>
-      </c>
-      <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="F15" s="13" t="e">
-        <f>IF(D15="",NA(),$F$5-SUM($D$6:D15))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G15" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>231</v>
-      </c>
-      <c r="B16">
-        <v>11</v>
-      </c>
-      <c r="F16" s="13" t="e">
-        <f>IF(D16="",NA(),$F$5-SUM($D$6:D16))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G16" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>232</v>
-      </c>
-      <c r="B17">
-        <v>12</v>
-      </c>
-      <c r="F17" s="13" t="e">
-        <f>IF(D17="",NA(),$F$5-SUM($D$6:D17))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G17" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18">
-        <v>13</v>
-      </c>
-      <c r="F18" s="13" t="e">
-        <f>IF(D18="",NA(),$F$5-SUM($D$6:D18))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G18" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>234</v>
-      </c>
-      <c r="B19">
-        <v>14</v>
-      </c>
-      <c r="F19" s="13" t="e">
-        <f>IF(D19="",NA(),$F$5-SUM($D$6:D19))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G19" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B20">
-        <v>15</v>
-      </c>
-      <c r="F20" s="13" t="e">
-        <f>IF(D20="",NA(),$F$5-SUM($D$6:D20))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G20" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>236</v>
-      </c>
-      <c r="B21">
-        <v>16</v>
-      </c>
-      <c r="F21" s="13" t="e">
-        <f>IF(D21="",NA(),$F$5-SUM($D$6:D21))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G21" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>237</v>
-      </c>
-      <c r="B22">
-        <v>17</v>
-      </c>
-      <c r="F22" s="13" t="e">
-        <f>IF(D22="",NA(),$F$5-SUM($D$6:D22))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G22" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>238</v>
-      </c>
-      <c r="B23">
-        <v>18</v>
-      </c>
-      <c r="F23" s="13" t="e">
-        <f>IF(D23="",NA(),$F$5-SUM($D$6:D23))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G23" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>239</v>
-      </c>
-      <c r="B24">
-        <v>19</v>
-      </c>
-      <c r="F24" s="13" t="e">
-        <f>IF(D24="",NA(),$F$5-SUM($D$6:D24))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G24" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>240</v>
-      </c>
-      <c r="B25">
-        <v>20</v>
-      </c>
-      <c r="F25" s="13" t="e">
-        <f>IF(D25="",NA(),$F$5-SUM($D$6:D25))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G25" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="17"/>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.45">
-      <c r="A33" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C38" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A15:G15"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
@@ -4003,23 +4166,23 @@
       <selection activeCell="A10" sqref="A10:K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="32.3984375" customWidth="1"/>
-    <col min="4" max="4" width="53.265625" customWidth="1"/>
-    <col min="5" max="5" width="26.73046875" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.3984375" customWidth="1"/>
-    <col min="8" max="8" width="17.1328125" customWidth="1"/>
-    <col min="9" max="9" width="18.1328125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="16.86328125" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4054,7 +4217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -4086,7 +4249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -4118,7 +4281,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -4150,7 +4313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1.4</v>
       </c>
@@ -4182,7 +4345,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1.5</v>
       </c>
@@ -4214,7 +4377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1.6</v>
       </c>
@@ -4246,7 +4409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1.7</v>
       </c>
@@ -4278,7 +4441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2.1</v>
       </c>
@@ -4310,7 +4473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2.2000000000000002</v>
       </c>
@@ -4342,7 +4505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>2.2999999999999998</v>
       </c>
@@ -4374,7 +4537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2.4</v>
       </c>
@@ -4406,7 +4569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2.5</v>
       </c>
@@ -4438,7 +4601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2.6</v>
       </c>
@@ -4470,7 +4633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>2.7</v>
       </c>
@@ -4502,7 +4665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>3.1</v>
       </c>
@@ -4534,7 +4697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>3.2</v>
       </c>
@@ -4566,7 +4729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>3.3</v>
       </c>
@@ -4598,7 +4761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>3.4</v>
       </c>
@@ -4630,8 +4793,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A22" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B22">
@@ -4662,8 +4825,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B23">
@@ -4694,7 +4857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>3.6</v>
       </c>
@@ -4726,7 +4889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>3.8</v>
       </c>
@@ -4758,7 +4921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>3.9</v>
       </c>

</xml_diff>